<commit_message>
SolarPACES2024 Rollout Cleaning Optimization study
Code used to generate SolarPACES 2024 rollout heuristic results
</commit_message>
<xml_diff>
--- a/woomera_demo/parameters.xlsx
+++ b/woomera_demo/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://connectqutedu-my.sharepoint.com/personal/cholette_qut_edu_au/Documents/ASTRI/python_soiling_model/HelioSoil/woomera_demo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cody Anderson\Offline\GitHub\HelioSoil\woomera_demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{F12345C8-0D5A-4BCB-8817-388D9958DC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAE3EC73-C232-494D-A840-20F6F8A922D9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD6E30C-A82B-4C77-BA37-FD868F8D9E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="16200" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -333,7 +333,7 @@
     <t>optical height of receiver tower</t>
   </si>
   <si>
-    <t>mie</t>
+    <t>geometry</t>
   </si>
 </sst>
 </file>
@@ -903,9 +903,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -943,7 +943,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1049,7 +1049,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1191,7 +1191,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1201,19 +1201,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFB43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.796875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="97.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="97.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1227,13 +1227,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1286,18 +1286,18 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="2">
-        <v>50</v>
+        <v>5.8</v>
       </c>
       <c r="D7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>94</v>
       </c>
@@ -1311,13 +1311,13 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>89</v>
       </c>
@@ -5454,7 +5454,7 @@
       <c r="XEX12" s="2"/>
       <c r="XFB12" s="2"/>
     </row>
-    <row r="13" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -5468,7 +5468,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -5482,7 +5482,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>92</v>
       </c>
@@ -5496,7 +5496,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1022 1026:2046 2050:3070 3074:4094 4098:5118 5122:6142 6146:7166 7170:8190 8194:9214 9218:10238 10242:11262 11266:12286 12290:13310 13314:14334 14338:15358 15362:16382" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -5510,7 +5510,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -5524,7 +5524,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -5538,7 +5538,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>82</v>
       </c>
@@ -5552,7 +5552,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -5566,13 +5566,13 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -5586,7 +5586,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -5600,7 +5600,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -5614,7 +5614,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -5628,7 +5628,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -5639,7 +5639,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -5653,13 +5653,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -5673,7 +5673,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -5687,7 +5687,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -5701,7 +5701,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -5715,7 +5715,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -5726,7 +5726,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -5740,7 +5740,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -5751,7 +5751,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -5762,7 +5762,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -5773,7 +5773,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -5784,7 +5784,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -5806,7 +5806,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -5817,7 +5817,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>55</v>
       </c>
@@ -5831,7 +5831,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>88</v>
       </c>

</xml_diff>